<commit_message>
Update Plotting top three algorithms.xlsx
</commit_message>
<xml_diff>
--- a/Working Implementation/Plotting top three algorithms.xlsx
+++ b/Working Implementation/Plotting top three algorithms.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simeo\Documents\GitHub\liboqs\Working Implementation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14FEFC0-6857-4017-B486-BD4716938436}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE38AC68-8996-4B1C-ACB4-D37B86280E3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{90DBE575-CC9A-43C6-B12F-2DFB5AB91FF6}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Data!$A$1:$L$64</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Data!$A$1:$L$62</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
   <si>
     <t>Name</t>
   </si>
@@ -263,12 +263,6 @@
   </si>
   <si>
     <t>picnic2_L5_FS</t>
-  </si>
-  <si>
-    <t>qTesla-p-I</t>
-  </si>
-  <si>
-    <t>qTesla-p-III</t>
   </si>
   <si>
     <t>Combined milliseconds</t>
@@ -401,11 +395,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$L$1</c:f>
+              <c:f>Data!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Combined milliseconds</c:v>
+                  <c:v>Key generation milliseconds</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -425,196 +419,190 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$A$2:$A$64</c:f>
+              <c:f>Data!$A$2:$A$62</c:f>
               <c:strCache>
-                <c:ptCount val="63"/>
+                <c:ptCount val="61"/>
                 <c:pt idx="0">
+                  <c:v>picnic_L1_UR</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>picnic_L1_FS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>picnic_L3_UR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>picnic_L3_FS</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>picnic_L5_FS</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>picnic_L5_UR</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>picnic2_L1_FS</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>picnic2_L3_FS</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>picnic2_L5_FS</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>DILITHIUM_2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="10">
+                  <c:v>DILITHIUM_3</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>DILITHIUM_4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>DILITHIUM_3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>qTesla-p-I</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>picnic_L1_FS</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>picnic_L1_UR</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>qTesla-p-III</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>SPHINCS+-Haraka-128f-simple</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>SPHINCS+-Haraka-128f-robust</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>picnic_L3_FS</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>SPHINCS+-Haraka-192f-simple</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>SPHINCS+-Haraka-192f-robust</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>MQDSS-31-48</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>picnic_L3_UR</c:v>
+                  <c:v>SPHINCS+-Haraka-128f-simple</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>Falcon-512</c:v>
+                  <c:v>SPHINCS+-Haraka-128f-robust</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>SPHINCS+-Haraka-192f-simple</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>SPHINCS+-Haraka-192f-robust</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>SPHINCS+-SHA256-128f-simple</c:v>
                 </c:pt>
-                <c:pt idx="16">
-                  <c:v>picnic_L5_FS</c:v>
-                </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
+                  <c:v>MQDSS-31-64</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>SPHINCS+-SHA256-192f-simple</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>picnic_L5_UR</c:v>
-                </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
+                  <c:v>SPHINCS+-SHA256-128f-robust</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>SPHINCS+-Haraka-256f-simple</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>SPHINCS+-Haraka-256f-robust</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>SPHINCS+-SHA256-128f-robust</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>SPHINCS+-SHAKE256-128f-simple</c:v>
                 </c:pt>
                 <c:pt idx="23">
+                  <c:v>SPHINCS+-Haraka-256f-robust</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>SPHINCS+-SHA256-192f-robust</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>SPHINCS+-SHAKE256-192f-simple</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>SPHINCS+-SHA256-256f-simple</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>SPHINCS+-SHAKE256-128f-robust</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>SPHINCS+-SHAKE256-192f-robust</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>SPHINCS+-SHAKE256-256f-simple</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>SPHINCS+-SHA256-256f-robust</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>SPHINCS+-SHAKE256-256f-robust</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>SPHINCS+-Haraka-128s-simple</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>SPHINCS+-Haraka-128s-robust</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Falcon-512</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>SPHINCS+-Haraka-192s-simple</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>SPHINCS+-Haraka-192s-robust</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>SPHINCS+-SHA256-128s-simple</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>SPHINCS+-Haraka-256s-simple</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>SPHINCS+-Haraka-256s-robust</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>SPHINCS+-SHA256-192s-simple</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>SPHINCS+-SHA256-256s-simple</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>SPHINCS+-SHA256-128s-robust</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>SPHINCS+-SHAKE256-128s-simple</c:v>
+                </c:pt>
+                <c:pt idx="44">
                   <c:v>Falcon-1024</c:v>
                 </c:pt>
-                <c:pt idx="24">
-                  <c:v>SPHINCS+-SHA256-256f-simple</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>MQDSS-31-64</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>SPHINCS+-SHA256-192f-robust</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>SPHINCS+-SHAKE256-192f-simple</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>SPHINCS+-SHAKE256-128f-robust</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>SPHINCS+-SHAKE256-192f-robust</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>SPHINCS+-SHAKE256-256f-simple</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>picnic2_L1_FS</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>SPHINCS+-SHA256-256f-robust</c:v>
-                </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="45">
+                  <c:v>SPHINCS+-SHA256-192s-robust</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>SPHINCS+-SHAKE256-192s-simple</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>SPHINCS+-SHAKE256-128s-robust</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>SPHINCS+-SHAKE256-256s-simple</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>SPHINCS+-SHA256-256s-robust</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>SPHINCS+-SHAKE256-192s-robust</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>SPHINCS+-SHAKE256-256s-robust</c:v>
+                </c:pt>
+                <c:pt idx="52">
                   <c:v>Rainbow-Ia-Classic</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="53">
+                  <c:v>Rainbow-Ia-Cyclic-Compressed</c:v>
+                </c:pt>
+                <c:pt idx="54">
                   <c:v>Rainbow-Ia-Cyclic</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>SPHINCS+-Haraka-128s-simple</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>SPHINCS+-SHAKE256-256f-robust</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>SPHINCS+-Haraka-128s-robust</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>Rainbow-Ia-Cyclic-Compressed</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>SPHINCS+-Haraka-256s-simple</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>SPHINCS+-SHA256-128s-simple</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>SPHINCS+-Haraka-256s-robust</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>SPHINCS+-Haraka-192s-simple</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>picnic2_L3_FS</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>SPHINCS+-SHA256-256s-simple</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>SPHINCS+-Haraka-192s-robust</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>SPHINCS+-SHA256-192s-simple</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>SPHINCS+-SHA256-128s-robust</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>SPHINCS+-SHAKE256-128s-simple</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>picnic2_L5_FS</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>SPHINCS+-SHAKE256-256s-simple</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>SPHINCS+-SHA256-192s-robust</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>SPHINCS+-SHAKE256-128s-robust</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>SPHINCS+-SHA256-256s-robust</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>SPHINCS+-SHAKE256-192s-simple</c:v>
                 </c:pt>
                 <c:pt idx="55">
                   <c:v>Rainbow-IIIc-Classic</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>SPHINCS+-SHAKE256-256s-robust</c:v>
+                  <c:v>Rainbow-IIIc-Cyclic-Compressed</c:v>
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>Rainbow-IIIc-Cyclic</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>SPHINCS+-SHAKE256-192s-robust</c:v>
+                  <c:v>Rainbow-Vc-Classic</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>Rainbow-IIIc-Cyclic-Compressed</c:v>
+                  <c:v>Rainbow-Vc-Cyclic</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>Rainbow-Vc-Classic</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>Rainbow-Vc-Cyclic</c:v>
-                </c:pt>
-                <c:pt idx="62">
                   <c:v>Rainbow-Vc-Cyclic-Compressed</c:v>
                 </c:pt>
               </c:strCache>
@@ -622,198 +610,192 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$L$2:$L$64</c:f>
+              <c:f>Data!$I$2:$I$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="63"/>
+                <c:ptCount val="61"/>
                 <c:pt idx="0">
-                  <c:v>0.98719999999999997</c:v>
+                  <c:v>5.5759999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3813899999999999</c:v>
+                  <c:v>5.62E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4540800000000003</c:v>
+                  <c:v>6.062E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.96367</c:v>
+                  <c:v>6.0690000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.0744100000000003</c:v>
+                  <c:v>6.5259999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.8286499999999997</c:v>
+                  <c:v>6.5310000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.8647900000000011</c:v>
+                  <c:v>6.9029999999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.238200000000001</c:v>
+                  <c:v>7.6740000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13.093219999999999</c:v>
+                  <c:v>8.1860000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14.022169999999999</c:v>
+                  <c:v>0.13457</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14.742140000000001</c:v>
+                  <c:v>0.18653</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16.51332</c:v>
+                  <c:v>0.22064</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>17.54766</c:v>
+                  <c:v>0.30886000000000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>18.56354</c:v>
+                  <c:v>0.37103999999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>19.41581</c:v>
+                  <c:v>0.38108999999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>22.544640000000001</c:v>
+                  <c:v>0.51520999999999995</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>23.935500000000001</c:v>
+                  <c:v>0.55437999999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>29.454549999999998</c:v>
+                  <c:v>0.56555999999999995</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>30.193660000000001</c:v>
+                  <c:v>0.66864000000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>30.92482</c:v>
+                  <c:v>0.75397999999999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>36.141959999999997</c:v>
+                  <c:v>1.0167900000000001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>40.245269999999998</c:v>
+                  <c:v>1.2055</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>48.227249999999998</c:v>
+                  <c:v>1.3146</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>51.611580000000004</c:v>
+                  <c:v>1.39402</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>55.05968</c:v>
+                  <c:v>1.4635400000000001</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>55.263010000000001</c:v>
+                  <c:v>1.92557</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>55.705440000000003</c:v>
+                  <c:v>1.9457100000000001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>63.257480000000001</c:v>
+                  <c:v>2.2859699999999998</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>82.222970000000004</c:v>
+                  <c:v>3.3480500000000002</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>110.54179999999999</c:v>
+                  <c:v>4.7530900000000003</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>123.78239000000001</c:v>
+                  <c:v>6.5458100000000004</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>158.70631</c:v>
+                  <c:v>8.3167899999999992</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>166.45819</c:v>
+                  <c:v>10.68638</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>172.95353999999998</c:v>
+                  <c:v>11.54612</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>183.94842</c:v>
+                  <c:v>14.866849999999999</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>192.01376999999999</c:v>
+                  <c:v>15.35557</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>212.14071000000001</c:v>
+                  <c:v>16.841699999999999</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>217.77656999999999</c:v>
+                  <c:v>16.85333</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>256.10534999999999</c:v>
+                  <c:v>20.01267</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>281.91674</c:v>
+                  <c:v>21.7898</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>314.46436</c:v>
+                  <c:v>23.675170000000001</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>317.85291000000001</c:v>
+                  <c:v>30.743670000000002</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>398.67566999999997</c:v>
+                  <c:v>32.254190000000001</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>401.07549999999998</c:v>
+                  <c:v>41.81</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>418.64708000000002</c:v>
+                  <c:v>41.837820000000001</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>467.03109000000001</c:v>
+                  <c:v>47.65502</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>576.05841999999996</c:v>
+                  <c:v>60.010210000000001</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>580.21711000000005</c:v>
+                  <c:v>71.863299999999995</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>700.60833000000002</c:v>
+                  <c:v>76.74239</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>776.2201</c:v>
+                  <c:v>104.81656</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1026.25792</c:v>
+                  <c:v>105.19821</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1056.6633200000001</c:v>
+                  <c:v>133.78276</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1150.1530700000001</c:v>
+                  <c:v>168.57817</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1314.94371</c:v>
+                  <c:v>178.06133</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1434.0514699999999</c:v>
+                  <c:v>179.50781000000001</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1571.6337600000002</c:v>
+                  <c:v>1543.49288</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1704.5694000000001</c:v>
+                  <c:v>1764.7177200000001</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1874.32809</c:v>
+                  <c:v>1842.2816399999999</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2313.7494999999999</c:v>
+                  <c:v>4935.3847699999997</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>2627.6624900000002</c:v>
+                  <c:v>5600.4545099999996</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>5001.9953399999995</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>5673.1250099999988</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>8327.5355400000008</c:v>
+                  <c:v>5610.2878499999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1531,16 +1513,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>676712</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19815</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>141449</xdr:rowOff>
+      <xdr:rowOff>163346</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>950310</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>98534</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>328449</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>120431</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1590,10 +1572,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89F39C01-0F6B-4737-AE7B-12FAFFC7BABE}" name="Algorithm_benchmark_100" displayName="Algorithm_benchmark_100" ref="A1:L64" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:L64" xr:uid="{B690E954-4B89-4B26-BD9D-A3922ACF1CFD}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L64">
-    <sortCondition ref="L1:L64"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89F39C01-0F6B-4737-AE7B-12FAFFC7BABE}" name="Algorithm_benchmark_100" displayName="Algorithm_benchmark_100" ref="A1:L62" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:L62" xr:uid="{B690E954-4B89-4B26-BD9D-A3922ACF1CFD}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L62">
+    <sortCondition ref="I1:I62"/>
   </sortState>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{52F44F0E-D916-42EC-B1CE-5A02F6B8F367}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="2"/>
@@ -1910,11 +1892,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08463C9E-C5B5-4188-BA39-46F88B5828AE}">
-  <dimension ref="A1:L64"/>
+  <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="87" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I2" sqref="A2:L62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1967,24 +1949,24 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="B2">
-        <v>1184</v>
+        <v>33</v>
       </c>
       <c r="C2">
-        <v>2800</v>
+        <v>49</v>
       </c>
       <c r="D2">
-        <v>2044</v>
+        <v>53965</v>
       </c>
       <c r="E2">
-        <v>3228</v>
+        <v>53998</v>
       </c>
       <c r="F2">
         <v>100</v>
@@ -1993,37 +1975,37 @@
         <v>12</v>
       </c>
       <c r="H2">
-        <v>2.8400000000000001E-3</v>
+        <v>3.3300000000000001E-3</v>
       </c>
       <c r="I2">
-        <v>0.13457</v>
+        <v>5.5759999999999997E-2</v>
       </c>
       <c r="J2">
-        <v>0.72589000000000004</v>
+        <v>4.3345099999999999</v>
       </c>
       <c r="K2">
-        <v>0.12673999999999999</v>
+        <v>3.43838</v>
       </c>
       <c r="L2" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>0.98719999999999997</v>
+        <v>7.8286499999999997</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="B3">
-        <v>1760</v>
+        <v>33</v>
       </c>
       <c r="C3">
-        <v>3856</v>
+        <v>49</v>
       </c>
       <c r="D3">
-        <v>3366</v>
+        <v>34036</v>
       </c>
       <c r="E3">
-        <v>5126</v>
+        <v>34069</v>
       </c>
       <c r="F3">
         <v>100</v>
@@ -2032,37 +2014,37 @@
         <v>12</v>
       </c>
       <c r="H3">
-        <v>4.3099999999999996E-3</v>
+        <v>3.5899999999999999E-3</v>
       </c>
       <c r="I3">
-        <v>0.22064</v>
+        <v>5.62E-2</v>
       </c>
       <c r="J3">
-        <v>0.93603999999999998</v>
+        <v>3.3733900000000001</v>
       </c>
       <c r="K3">
-        <v>0.22470999999999999</v>
+        <v>2.6448200000000002</v>
       </c>
       <c r="L3" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>1.3813899999999999</v>
+        <v>6.0744100000000003</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="B4">
-        <v>1472</v>
+        <v>49</v>
       </c>
       <c r="C4">
-        <v>3504</v>
+        <v>73</v>
       </c>
       <c r="D4">
-        <v>2701</v>
+        <v>121849</v>
       </c>
       <c r="E4">
-        <v>4173</v>
+        <v>121898</v>
       </c>
       <c r="F4">
         <v>100</v>
@@ -2071,37 +2053,37 @@
         <v>12</v>
       </c>
       <c r="H4">
-        <v>3.7200000000000002E-3</v>
+        <v>4.1200000000000004E-3</v>
       </c>
       <c r="I4">
-        <v>0.18653</v>
+        <v>6.062E-2</v>
       </c>
       <c r="J4">
-        <v>1.0958600000000001</v>
+        <v>10.2638</v>
       </c>
       <c r="K4">
-        <v>0.17169000000000001</v>
+        <v>8.2391199999999998</v>
       </c>
       <c r="L4" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>1.4540800000000003</v>
+        <v>18.56354</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5">
+        <v>49</v>
+      </c>
+      <c r="C5">
         <v>73</v>
       </c>
-      <c r="B5">
-        <v>14880</v>
-      </c>
-      <c r="C5">
-        <v>5224</v>
-      </c>
       <c r="D5">
-        <v>2592</v>
+        <v>76776</v>
       </c>
       <c r="E5">
-        <v>17472</v>
+        <v>76825</v>
       </c>
       <c r="F5">
         <v>100</v>
@@ -2110,37 +2092,37 @@
         <v>12</v>
       </c>
       <c r="H5">
-        <v>3.98E-3</v>
+        <v>3.63E-3</v>
       </c>
       <c r="I5">
-        <v>0.89078000000000002</v>
+        <v>6.0690000000000001E-2</v>
       </c>
       <c r="J5">
-        <v>0.80632999999999999</v>
+        <v>7.7017199999999999</v>
       </c>
       <c r="K5">
-        <v>0.26656000000000002</v>
+        <v>6.25976</v>
       </c>
       <c r="L5" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>1.96367</v>
+        <v>14.022169999999999</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B6">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="C6">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="D6">
-        <v>34036</v>
+        <v>132860</v>
       </c>
       <c r="E6">
-        <v>34069</v>
+        <v>132925</v>
       </c>
       <c r="F6">
         <v>100</v>
@@ -2149,37 +2131,37 @@
         <v>12</v>
       </c>
       <c r="H6">
-        <v>3.5899999999999999E-3</v>
+        <v>3.79E-3</v>
       </c>
       <c r="I6">
-        <v>5.62E-2</v>
+        <v>6.5259999999999999E-2</v>
       </c>
       <c r="J6">
-        <v>3.3733900000000001</v>
+        <v>13.11078</v>
       </c>
       <c r="K6">
-        <v>2.6448200000000002</v>
+        <v>10.759460000000001</v>
       </c>
       <c r="L6" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>6.0744100000000003</v>
+        <v>23.935500000000001</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7">
         <v>65</v>
       </c>
-      <c r="B7">
-        <v>33</v>
-      </c>
       <c r="C7">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="D7">
-        <v>53965</v>
+        <v>209510</v>
       </c>
       <c r="E7">
-        <v>53998</v>
+        <v>209575</v>
       </c>
       <c r="F7">
         <v>100</v>
@@ -2188,37 +2170,37 @@
         <v>12</v>
       </c>
       <c r="H7">
-        <v>3.3300000000000001E-3</v>
+        <v>4.7299999999999998E-3</v>
       </c>
       <c r="I7">
-        <v>5.5759999999999997E-2</v>
+        <v>6.5310000000000007E-2</v>
       </c>
       <c r="J7">
-        <v>4.3345099999999999</v>
+        <v>16.613209999999999</v>
       </c>
       <c r="K7">
-        <v>3.43838</v>
+        <v>13.515140000000001</v>
       </c>
       <c r="L7" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>7.8286499999999997</v>
+        <v>30.193660000000001</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B8">
-        <v>38432</v>
+        <v>33</v>
       </c>
       <c r="C8">
-        <v>12392</v>
+        <v>49</v>
       </c>
       <c r="D8">
-        <v>5664</v>
+        <v>13806</v>
       </c>
       <c r="E8">
-        <v>44096</v>
+        <v>13839</v>
       </c>
       <c r="F8">
         <v>100</v>
@@ -2227,37 +2209,37 @@
         <v>12</v>
       </c>
       <c r="H8">
-        <v>4.1700000000000001E-3</v>
+        <v>4.8799999999999998E-3</v>
       </c>
       <c r="I8">
-        <v>5.0709400000000002</v>
+        <v>6.9029999999999994E-2</v>
       </c>
       <c r="J8">
-        <v>2.0956100000000002</v>
+        <v>103.4233</v>
       </c>
       <c r="K8">
-        <v>0.69823999999999997</v>
+        <v>55.213979999999999</v>
       </c>
       <c r="L8" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>7.8647900000000011</v>
+        <v>158.70631</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="B9">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C9">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="D9">
-        <v>16976</v>
+        <v>29754</v>
       </c>
       <c r="E9">
-        <v>17008</v>
+        <v>29803</v>
       </c>
       <c r="F9">
         <v>100</v>
@@ -2266,37 +2248,37 @@
         <v>12</v>
       </c>
       <c r="H9">
-        <v>2.33E-3</v>
+        <v>5.45E-3</v>
       </c>
       <c r="I9">
-        <v>0.37103999999999998</v>
+        <v>7.6740000000000003E-2</v>
       </c>
       <c r="J9">
-        <v>11.39561</v>
+        <v>280.47131999999999</v>
       </c>
       <c r="K9">
-        <v>0.47155000000000002</v>
+        <v>120.52744</v>
       </c>
       <c r="L9" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>12.238200000000001</v>
+        <v>401.07549999999998</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="B10">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="C10">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="D10">
-        <v>16976</v>
+        <v>54736</v>
       </c>
       <c r="E10">
-        <v>17008</v>
+        <v>54801</v>
       </c>
       <c r="F10">
         <v>100</v>
@@ -2305,37 +2287,37 @@
         <v>12</v>
       </c>
       <c r="H10">
-        <v>2.33E-3</v>
+        <v>6.0200000000000002E-3</v>
       </c>
       <c r="I10">
-        <v>0.38108999999999998</v>
+        <v>8.1860000000000002E-2</v>
       </c>
       <c r="J10">
-        <v>12.228579999999999</v>
+        <v>565.85675000000003</v>
       </c>
       <c r="K10">
-        <v>0.48354999999999998</v>
+        <v>210.28148999999999</v>
       </c>
       <c r="L10" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>13.093219999999999</v>
+        <v>776.2201</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="B11">
-        <v>49</v>
+        <v>1184</v>
       </c>
       <c r="C11">
-        <v>73</v>
+        <v>2800</v>
       </c>
       <c r="D11">
-        <v>76776</v>
+        <v>2044</v>
       </c>
       <c r="E11">
-        <v>76825</v>
+        <v>3228</v>
       </c>
       <c r="F11">
         <v>100</v>
@@ -2344,37 +2326,37 @@
         <v>12</v>
       </c>
       <c r="H11">
-        <v>3.63E-3</v>
+        <v>2.8400000000000001E-3</v>
       </c>
       <c r="I11">
-        <v>6.0690000000000001E-2</v>
+        <v>0.13457</v>
       </c>
       <c r="J11">
-        <v>7.7017199999999999</v>
+        <v>0.72589000000000004</v>
       </c>
       <c r="K11">
-        <v>6.25976</v>
+        <v>0.12673999999999999</v>
       </c>
       <c r="L11" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>14.022169999999999</v>
+        <v>0.98719999999999997</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="B12">
-        <v>48</v>
+        <v>1472</v>
       </c>
       <c r="C12">
-        <v>96</v>
+        <v>3504</v>
       </c>
       <c r="D12">
-        <v>35664</v>
+        <v>2701</v>
       </c>
       <c r="E12">
-        <v>35712</v>
+        <v>4173</v>
       </c>
       <c r="F12">
         <v>100</v>
@@ -2383,37 +2365,37 @@
         <v>12</v>
       </c>
       <c r="H12">
-        <v>2.64E-3</v>
+        <v>3.7200000000000002E-3</v>
       </c>
       <c r="I12">
-        <v>0.51520999999999995</v>
+        <v>0.18653</v>
       </c>
       <c r="J12">
-        <v>13.52908</v>
+        <v>1.0958600000000001</v>
       </c>
       <c r="K12">
-        <v>0.69784999999999997</v>
+        <v>0.17169000000000001</v>
       </c>
       <c r="L12" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>14.742140000000001</v>
+        <v>1.4540800000000003</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B13">
-        <v>48</v>
+        <v>1760</v>
       </c>
       <c r="C13">
-        <v>96</v>
+        <v>3856</v>
       </c>
       <c r="D13">
-        <v>35664</v>
+        <v>3366</v>
       </c>
       <c r="E13">
-        <v>35712</v>
+        <v>5126</v>
       </c>
       <c r="F13">
         <v>100</v>
@@ -2422,20 +2404,20 @@
         <v>12</v>
       </c>
       <c r="H13">
-        <v>2.5899999999999999E-3</v>
+        <v>4.3099999999999996E-3</v>
       </c>
       <c r="I13">
-        <v>0.55437999999999998</v>
+        <v>0.22064</v>
       </c>
       <c r="J13">
-        <v>15.16986</v>
+        <v>0.93603999999999998</v>
       </c>
       <c r="K13">
-        <v>0.78908</v>
+        <v>0.22470999999999999</v>
       </c>
       <c r="L13" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>16.51332</v>
+        <v>1.3813899999999999</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2479,19 +2461,19 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="B15">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C15">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D15">
-        <v>121849</v>
+        <v>16976</v>
       </c>
       <c r="E15">
-        <v>121898</v>
+        <v>17008</v>
       </c>
       <c r="F15">
         <v>100</v>
@@ -2500,37 +2482,37 @@
         <v>12</v>
       </c>
       <c r="H15">
-        <v>4.1200000000000004E-3</v>
+        <v>2.33E-3</v>
       </c>
       <c r="I15">
-        <v>6.062E-2</v>
+        <v>0.37103999999999998</v>
       </c>
       <c r="J15">
-        <v>10.2638</v>
+        <v>11.39561</v>
       </c>
       <c r="K15">
-        <v>8.2391199999999998</v>
+        <v>0.47155000000000002</v>
       </c>
       <c r="L15" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>18.56354</v>
+        <v>12.238200000000001</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B16">
-        <v>897</v>
+        <v>32</v>
       </c>
       <c r="C16">
-        <v>1281</v>
+        <v>64</v>
       </c>
       <c r="D16">
-        <v>690</v>
+        <v>16976</v>
       </c>
       <c r="E16">
-        <v>1587</v>
+        <v>17008</v>
       </c>
       <c r="F16">
         <v>100</v>
@@ -2539,37 +2521,37 @@
         <v>12</v>
       </c>
       <c r="H16">
-        <v>1.56E-3</v>
+        <v>2.33E-3</v>
       </c>
       <c r="I16">
-        <v>14.866849999999999</v>
+        <v>0.38108999999999998</v>
       </c>
       <c r="J16">
-        <v>4.5000900000000001</v>
+        <v>12.228579999999999</v>
       </c>
       <c r="K16">
-        <v>4.8869999999999997E-2</v>
+        <v>0.48354999999999998</v>
       </c>
       <c r="L16" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>19.41581</v>
+        <v>13.093219999999999</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B17">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C17">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="D17">
-        <v>16976</v>
+        <v>35664</v>
       </c>
       <c r="E17">
-        <v>17008</v>
+        <v>35712</v>
       </c>
       <c r="F17">
         <v>100</v>
@@ -2578,37 +2560,37 @@
         <v>12</v>
       </c>
       <c r="H17">
-        <v>3.1700000000000001E-3</v>
+        <v>2.64E-3</v>
       </c>
       <c r="I17">
-        <v>0.56555999999999995</v>
+        <v>0.51520999999999995</v>
       </c>
       <c r="J17">
-        <v>18.91394</v>
+        <v>13.52908</v>
       </c>
       <c r="K17">
-        <v>3.06514</v>
+        <v>0.69784999999999997</v>
       </c>
       <c r="L17" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>22.544640000000001</v>
+        <v>14.742140000000001</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="B18">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="C18">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D18">
-        <v>132860</v>
+        <v>35664</v>
       </c>
       <c r="E18">
-        <v>132925</v>
+        <v>35712</v>
       </c>
       <c r="F18">
         <v>100</v>
@@ -2617,37 +2599,37 @@
         <v>12</v>
       </c>
       <c r="H18">
-        <v>3.79E-3</v>
+        <v>2.5899999999999999E-3</v>
       </c>
       <c r="I18">
-        <v>6.5259999999999999E-2</v>
+        <v>0.55437999999999998</v>
       </c>
       <c r="J18">
-        <v>13.11078</v>
+        <v>15.16986</v>
       </c>
       <c r="K18">
-        <v>10.759460000000001</v>
+        <v>0.78908</v>
       </c>
       <c r="L18" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>23.935500000000001</v>
+        <v>16.51332</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B19">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C19">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="D19">
-        <v>35664</v>
+        <v>16976</v>
       </c>
       <c r="E19">
-        <v>35712</v>
+        <v>17008</v>
       </c>
       <c r="F19">
         <v>100</v>
@@ -2656,37 +2638,37 @@
         <v>12</v>
       </c>
       <c r="H19">
-        <v>3.32E-3</v>
+        <v>3.1700000000000001E-3</v>
       </c>
       <c r="I19">
-        <v>0.75397999999999998</v>
+        <v>0.56555999999999995</v>
       </c>
       <c r="J19">
-        <v>24.08297</v>
+        <v>18.91394</v>
       </c>
       <c r="K19">
-        <v>4.6176000000000004</v>
+        <v>3.06514</v>
       </c>
       <c r="L19" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>29.454549999999998</v>
+        <v>22.544640000000001</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>69</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20">
-        <v>97</v>
+        <v>24</v>
       </c>
       <c r="D20">
-        <v>209510</v>
+        <v>59928</v>
       </c>
       <c r="E20">
-        <v>209575</v>
+        <v>59992</v>
       </c>
       <c r="F20">
         <v>100</v>
@@ -2695,37 +2677,37 @@
         <v>12</v>
       </c>
       <c r="H20">
-        <v>4.7299999999999998E-3</v>
+        <v>2.3400000000000001E-3</v>
       </c>
       <c r="I20">
-        <v>6.5310000000000007E-2</v>
+        <v>0.66864000000000001</v>
       </c>
       <c r="J20">
-        <v>16.613209999999999</v>
+        <v>31.37229</v>
       </c>
       <c r="K20">
-        <v>13.515140000000001</v>
+        <v>23.222079999999998</v>
       </c>
       <c r="L20" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>30.193660000000001</v>
+        <v>55.263010000000001</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B21">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="C21">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="D21">
-        <v>49216</v>
+        <v>35664</v>
       </c>
       <c r="E21">
-        <v>49280</v>
+        <v>35712</v>
       </c>
       <c r="F21">
         <v>100</v>
@@ -2734,37 +2716,37 @@
         <v>12</v>
       </c>
       <c r="H21">
-        <v>3.15E-3</v>
+        <v>3.32E-3</v>
       </c>
       <c r="I21">
-        <v>1.2055</v>
+        <v>0.75397999999999998</v>
       </c>
       <c r="J21">
-        <v>29.01942</v>
+        <v>24.08297</v>
       </c>
       <c r="K21">
-        <v>0.69989999999999997</v>
+        <v>4.6176000000000004</v>
       </c>
       <c r="L21" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>30.92482</v>
+        <v>29.454549999999998</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B22">
+        <v>32</v>
+      </c>
+      <c r="C22">
         <v>64</v>
       </c>
-      <c r="C22">
-        <v>128</v>
-      </c>
       <c r="D22">
-        <v>49216</v>
+        <v>16976</v>
       </c>
       <c r="E22">
-        <v>49280</v>
+        <v>17008</v>
       </c>
       <c r="F22">
         <v>100</v>
@@ -2773,37 +2755,37 @@
         <v>12</v>
       </c>
       <c r="H22">
-        <v>3.13E-3</v>
+        <v>3.15E-3</v>
       </c>
       <c r="I22">
-        <v>1.39402</v>
+        <v>1.0167900000000001</v>
       </c>
       <c r="J22">
-        <v>33.949199999999998</v>
+        <v>33.644629999999999</v>
       </c>
       <c r="K22">
-        <v>0.79874000000000001</v>
+        <v>5.58385</v>
       </c>
       <c r="L22" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>36.141959999999997</v>
+        <v>40.245269999999998</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B23">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="C23">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="D23">
-        <v>16976</v>
+        <v>49216</v>
       </c>
       <c r="E23">
-        <v>17008</v>
+        <v>49280</v>
       </c>
       <c r="F23">
         <v>100</v>
@@ -2815,17 +2797,17 @@
         <v>3.15E-3</v>
       </c>
       <c r="I23">
-        <v>1.0167900000000001</v>
+        <v>1.2055</v>
       </c>
       <c r="J23">
-        <v>33.644629999999999</v>
+        <v>29.01942</v>
       </c>
       <c r="K23">
-        <v>5.58385</v>
+        <v>0.69989999999999997</v>
       </c>
       <c r="L23" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>40.245269999999998</v>
+        <v>30.92482</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -2869,19 +2851,19 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B25">
-        <v>1793</v>
+        <v>64</v>
       </c>
       <c r="C25">
-        <v>2305</v>
+        <v>128</v>
       </c>
       <c r="D25">
-        <v>1330</v>
+        <v>49216</v>
       </c>
       <c r="E25">
-        <v>3123</v>
+        <v>49280</v>
       </c>
       <c r="F25">
         <v>100</v>
@@ -2890,37 +2872,37 @@
         <v>12</v>
       </c>
       <c r="H25">
-        <v>1.8799999999999999E-3</v>
+        <v>3.13E-3</v>
       </c>
       <c r="I25">
-        <v>41.837820000000001</v>
+        <v>1.39402</v>
       </c>
       <c r="J25">
-        <v>9.6831999999999994</v>
+        <v>33.949199999999998</v>
       </c>
       <c r="K25">
-        <v>9.0560000000000002E-2</v>
+        <v>0.79874000000000001</v>
       </c>
       <c r="L25" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>51.611580000000004</v>
+        <v>36.141959999999997</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B26">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="C26">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="D26">
-        <v>49216</v>
+        <v>35664</v>
       </c>
       <c r="E26">
-        <v>49280</v>
+        <v>35712</v>
       </c>
       <c r="F26">
         <v>100</v>
@@ -2929,37 +2911,37 @@
         <v>12</v>
       </c>
       <c r="H26">
-        <v>3.8700000000000002E-3</v>
+        <v>3.8300000000000001E-3</v>
       </c>
       <c r="I26">
-        <v>1.9457100000000001</v>
+        <v>1.4635400000000001</v>
       </c>
       <c r="J26">
-        <v>48.417369999999998</v>
+        <v>45.40925</v>
       </c>
       <c r="K26">
-        <v>4.6966000000000001</v>
+        <v>8.8326499999999992</v>
       </c>
       <c r="L26" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>55.05968</v>
+        <v>55.705440000000003</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="B27">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="C27">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="D27">
-        <v>59928</v>
+        <v>35664</v>
       </c>
       <c r="E27">
-        <v>59992</v>
+        <v>35712</v>
       </c>
       <c r="F27">
         <v>100</v>
@@ -2968,37 +2950,37 @@
         <v>12</v>
       </c>
       <c r="H27">
-        <v>2.3400000000000001E-3</v>
+        <v>4.5300000000000002E-3</v>
       </c>
       <c r="I27">
-        <v>0.66864000000000001</v>
+        <v>1.92557</v>
       </c>
       <c r="J27">
-        <v>31.37229</v>
+        <v>55.361780000000003</v>
       </c>
       <c r="K27">
-        <v>23.222079999999998</v>
+        <v>5.9701300000000002</v>
       </c>
       <c r="L27" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>55.263010000000001</v>
+        <v>63.257480000000001</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B28">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C28">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="D28">
-        <v>35664</v>
+        <v>49216</v>
       </c>
       <c r="E28">
-        <v>35712</v>
+        <v>49280</v>
       </c>
       <c r="F28">
         <v>100</v>
@@ -3007,37 +2989,37 @@
         <v>12</v>
       </c>
       <c r="H28">
-        <v>3.8300000000000001E-3</v>
+        <v>3.8700000000000002E-3</v>
       </c>
       <c r="I28">
-        <v>1.4635400000000001</v>
+        <v>1.9457100000000001</v>
       </c>
       <c r="J28">
-        <v>45.40925</v>
+        <v>48.417369999999998</v>
       </c>
       <c r="K28">
-        <v>8.8326499999999992</v>
+        <v>4.6966000000000001</v>
       </c>
       <c r="L28" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>55.705440000000003</v>
+        <v>55.05968</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B29">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C29">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="D29">
-        <v>35664</v>
+        <v>16976</v>
       </c>
       <c r="E29">
-        <v>35712</v>
+        <v>17008</v>
       </c>
       <c r="F29">
         <v>100</v>
@@ -3046,37 +3028,37 @@
         <v>12</v>
       </c>
       <c r="H29">
-        <v>4.5300000000000002E-3</v>
+        <v>4.2399999999999998E-3</v>
       </c>
       <c r="I29">
-        <v>1.92557</v>
+        <v>2.2859699999999998</v>
       </c>
       <c r="J29">
-        <v>55.361780000000003</v>
+        <v>72.640979999999999</v>
       </c>
       <c r="K29">
-        <v>5.9701300000000002</v>
+        <v>7.2960200000000004</v>
       </c>
       <c r="L29" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>63.257480000000001</v>
+        <v>82.222970000000004</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B30">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C30">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="D30">
-        <v>16976</v>
+        <v>35664</v>
       </c>
       <c r="E30">
-        <v>17008</v>
+        <v>35712</v>
       </c>
       <c r="F30">
         <v>100</v>
@@ -3085,37 +3067,37 @@
         <v>12</v>
       </c>
       <c r="H30">
-        <v>4.2399999999999998E-3</v>
+        <v>4.5599999999999998E-3</v>
       </c>
       <c r="I30">
-        <v>2.2859699999999998</v>
+        <v>3.3480500000000002</v>
       </c>
       <c r="J30">
-        <v>72.640979999999999</v>
+        <v>95.801169999999999</v>
       </c>
       <c r="K30">
-        <v>7.2960200000000004</v>
+        <v>11.392580000000001</v>
       </c>
       <c r="L30" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>82.222970000000004</v>
+        <v>110.54179999999999</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B31">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C31">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="D31">
-        <v>35664</v>
+        <v>49216</v>
       </c>
       <c r="E31">
-        <v>35712</v>
+        <v>49280</v>
       </c>
       <c r="F31">
         <v>100</v>
@@ -3124,25 +3106,25 @@
         <v>12</v>
       </c>
       <c r="H31">
-        <v>4.5599999999999998E-3</v>
+        <v>5.0699999999999999E-3</v>
       </c>
       <c r="I31">
-        <v>3.3480500000000002</v>
+        <v>4.7530900000000003</v>
       </c>
       <c r="J31">
-        <v>95.801169999999999</v>
+        <v>113.09695000000001</v>
       </c>
       <c r="K31">
-        <v>11.392580000000001</v>
+        <v>5.9323499999999996</v>
       </c>
       <c r="L31" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>110.54179999999999</v>
+        <v>123.78239000000001</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B32">
         <v>64</v>
@@ -3163,37 +3145,37 @@
         <v>12</v>
       </c>
       <c r="H32">
-        <v>5.0699999999999999E-3</v>
+        <v>4.9100000000000003E-3</v>
       </c>
       <c r="I32">
-        <v>4.7530900000000003</v>
+        <v>6.5458100000000004</v>
       </c>
       <c r="J32">
-        <v>113.09695000000001</v>
+        <v>149.43010000000001</v>
       </c>
       <c r="K32">
-        <v>5.9323499999999996</v>
+        <v>10.482279999999999</v>
       </c>
       <c r="L32" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>123.78239000000001</v>
+        <v>166.45819</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B33">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="C33">
-        <v>49</v>
+        <v>128</v>
       </c>
       <c r="D33">
-        <v>13806</v>
+        <v>49216</v>
       </c>
       <c r="E33">
-        <v>13839</v>
+        <v>49280</v>
       </c>
       <c r="F33">
         <v>100</v>
@@ -3202,37 +3184,37 @@
         <v>12</v>
       </c>
       <c r="H33">
-        <v>4.8799999999999998E-3</v>
+        <v>5.5399999999999998E-3</v>
       </c>
       <c r="I33">
-        <v>6.9029999999999994E-2</v>
+        <v>8.3167899999999992</v>
       </c>
       <c r="J33">
-        <v>103.4233</v>
+        <v>192.24323000000001</v>
       </c>
       <c r="K33">
-        <v>55.213979999999999</v>
+        <v>11.580690000000001</v>
       </c>
       <c r="L33" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>158.70631</v>
+        <v>212.14071000000001</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B34">
+        <v>32</v>
+      </c>
+      <c r="C34">
         <v>64</v>
       </c>
-      <c r="C34">
-        <v>128</v>
-      </c>
       <c r="D34">
-        <v>49216</v>
+        <v>8080</v>
       </c>
       <c r="E34">
-        <v>49280</v>
+        <v>8112</v>
       </c>
       <c r="F34">
         <v>100</v>
@@ -3241,37 +3223,37 @@
         <v>12</v>
       </c>
       <c r="H34">
-        <v>4.9100000000000003E-3</v>
+        <v>4.2599999999999999E-3</v>
       </c>
       <c r="I34">
-        <v>6.5458100000000004</v>
+        <v>10.68638</v>
       </c>
       <c r="J34">
-        <v>149.43010000000001</v>
+        <v>181.13220000000001</v>
       </c>
       <c r="K34">
-        <v>10.482279999999999</v>
+        <v>0.19519</v>
       </c>
       <c r="L34" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>166.45819</v>
+        <v>192.01376999999999</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B35">
-        <v>148992</v>
+        <v>32</v>
       </c>
       <c r="C35">
-        <v>92960</v>
+        <v>64</v>
       </c>
       <c r="D35">
-        <v>64</v>
+        <v>8080</v>
       </c>
       <c r="E35">
-        <v>149056</v>
+        <v>8112</v>
       </c>
       <c r="F35">
         <v>100</v>
@@ -3280,37 +3262,37 @@
         <v>12</v>
       </c>
       <c r="H35">
-        <v>1.3610000000000001E-2</v>
+        <v>4.0699999999999998E-3</v>
       </c>
       <c r="I35">
-        <v>168.57817</v>
+        <v>11.54612</v>
       </c>
       <c r="J35">
-        <v>2.1260400000000002</v>
+        <v>206.00581</v>
       </c>
       <c r="K35">
-        <v>2.2493300000000001</v>
+        <v>0.22464000000000001</v>
       </c>
       <c r="L35" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>172.95353999999998</v>
+        <v>217.77656999999999</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B36">
-        <v>58144</v>
+        <v>897</v>
       </c>
       <c r="C36">
-        <v>92960</v>
+        <v>1281</v>
       </c>
       <c r="D36">
-        <v>64</v>
+        <v>690</v>
       </c>
       <c r="E36">
-        <v>58208</v>
+        <v>1587</v>
       </c>
       <c r="F36">
         <v>100</v>
@@ -3319,37 +3301,37 @@
         <v>12</v>
       </c>
       <c r="H36">
-        <v>1.2460000000000001E-2</v>
+        <v>1.56E-3</v>
       </c>
       <c r="I36">
-        <v>179.50781000000001</v>
+        <v>14.866849999999999</v>
       </c>
       <c r="J36">
-        <v>1.95381</v>
+        <v>4.5000900000000001</v>
       </c>
       <c r="K36">
-        <v>2.4868000000000001</v>
+        <v>4.8869999999999997E-2</v>
       </c>
       <c r="L36" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>183.94842</v>
+        <v>19.41581</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B37">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C37">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="D37">
-        <v>8080</v>
+        <v>17064</v>
       </c>
       <c r="E37">
-        <v>8112</v>
+        <v>17112</v>
       </c>
       <c r="F37">
         <v>100</v>
@@ -3358,37 +3340,37 @@
         <v>12</v>
       </c>
       <c r="H37">
-        <v>4.2599999999999999E-3</v>
+        <v>5.11E-3</v>
       </c>
       <c r="I37">
-        <v>10.68638</v>
+        <v>15.35557</v>
       </c>
       <c r="J37">
-        <v>181.13220000000001</v>
+        <v>383.04442999999998</v>
       </c>
       <c r="K37">
-        <v>0.19519</v>
+        <v>0.27567000000000003</v>
       </c>
       <c r="L37" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>192.01376999999999</v>
+        <v>398.67566999999997</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="B38">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="C38">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="D38">
-        <v>49216</v>
+        <v>17064</v>
       </c>
       <c r="E38">
-        <v>49280</v>
+        <v>17112</v>
       </c>
       <c r="F38">
         <v>100</v>
@@ -3397,25 +3379,25 @@
         <v>12</v>
       </c>
       <c r="H38">
-        <v>5.5399999999999998E-3</v>
+        <v>4.9300000000000004E-3</v>
       </c>
       <c r="I38">
-        <v>8.3167899999999992</v>
+        <v>16.841699999999999</v>
       </c>
       <c r="J38">
-        <v>192.24323000000001</v>
+        <v>449.87601999999998</v>
       </c>
       <c r="K38">
-        <v>11.580690000000001</v>
+        <v>0.31336999999999998</v>
       </c>
       <c r="L38" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>212.14071000000001</v>
+        <v>467.03109000000001</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B39">
         <v>32</v>
@@ -3436,37 +3418,37 @@
         <v>12</v>
       </c>
       <c r="H39">
-        <v>4.0699999999999998E-3</v>
+        <v>5.4900000000000001E-3</v>
       </c>
       <c r="I39">
-        <v>11.54612</v>
+        <v>16.85333</v>
       </c>
       <c r="J39">
-        <v>206.00581</v>
+        <v>296.37401999999997</v>
       </c>
       <c r="K39">
-        <v>0.22464000000000001</v>
+        <v>1.2370099999999999</v>
       </c>
       <c r="L39" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>217.77656999999999</v>
+        <v>314.46436</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B40">
-        <v>58144</v>
+        <v>64</v>
       </c>
       <c r="C40">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="D40">
-        <v>64</v>
+        <v>29792</v>
       </c>
       <c r="E40">
-        <v>58208</v>
+        <v>29856</v>
       </c>
       <c r="F40">
         <v>100</v>
@@ -3475,25 +3457,25 @@
         <v>12</v>
       </c>
       <c r="H40">
-        <v>1.048E-2</v>
+        <v>5.0400000000000002E-3</v>
       </c>
       <c r="I40">
-        <v>178.06133</v>
+        <v>20.01267</v>
       </c>
       <c r="J40">
-        <v>75.439949999999996</v>
+        <v>261.53915999999998</v>
       </c>
       <c r="K40">
-        <v>2.6040700000000001</v>
+        <v>0.36491000000000001</v>
       </c>
       <c r="L40" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>256.10534999999999</v>
+        <v>281.91674</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41">
         <v>64</v>
@@ -3514,37 +3496,37 @@
         <v>12</v>
       </c>
       <c r="H41">
-        <v>5.0400000000000002E-3</v>
+        <v>4.9100000000000003E-3</v>
       </c>
       <c r="I41">
-        <v>20.01267</v>
+        <v>21.7898</v>
       </c>
       <c r="J41">
-        <v>261.53915999999998</v>
+        <v>295.65107999999998</v>
       </c>
       <c r="K41">
-        <v>0.36491000000000001</v>
+        <v>0.41203000000000001</v>
       </c>
       <c r="L41" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>281.91674</v>
+        <v>317.85291000000001</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B42">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C42">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="D42">
-        <v>8080</v>
+        <v>17064</v>
       </c>
       <c r="E42">
-        <v>8112</v>
+        <v>17112</v>
       </c>
       <c r="F42">
         <v>100</v>
@@ -3553,25 +3535,25 @@
         <v>12</v>
       </c>
       <c r="H42">
-        <v>5.4900000000000001E-3</v>
+        <v>6.0600000000000003E-3</v>
       </c>
       <c r="I42">
-        <v>16.85333</v>
+        <v>23.675170000000001</v>
       </c>
       <c r="J42">
-        <v>296.37401999999997</v>
+        <v>550.56377999999995</v>
       </c>
       <c r="K42">
-        <v>1.2370099999999999</v>
+        <v>1.8194699999999999</v>
       </c>
       <c r="L42" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>314.46436</v>
+        <v>576.05841999999996</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B43">
         <v>64</v>
@@ -3592,37 +3574,37 @@
         <v>12</v>
       </c>
       <c r="H43">
-        <v>4.9100000000000003E-3</v>
+        <v>6.1399999999999996E-3</v>
       </c>
       <c r="I43">
-        <v>21.7898</v>
+        <v>30.743670000000002</v>
       </c>
       <c r="J43">
-        <v>295.65107999999998</v>
+        <v>385.53147000000001</v>
       </c>
       <c r="K43">
-        <v>0.41203000000000001</v>
+        <v>2.3719399999999999</v>
       </c>
       <c r="L43" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>317.85291000000001</v>
+        <v>418.64708000000002</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B44">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C44">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="D44">
-        <v>17064</v>
+        <v>8080</v>
       </c>
       <c r="E44">
-        <v>17112</v>
+        <v>8112</v>
       </c>
       <c r="F44">
         <v>100</v>
@@ -3631,37 +3613,37 @@
         <v>12</v>
       </c>
       <c r="H44">
-        <v>5.11E-3</v>
+        <v>5.2199999999999998E-3</v>
       </c>
       <c r="I44">
-        <v>15.35557</v>
+        <v>32.254190000000001</v>
       </c>
       <c r="J44">
-        <v>383.04442999999998</v>
+        <v>545.66493000000003</v>
       </c>
       <c r="K44">
-        <v>0.27567000000000003</v>
+        <v>2.29799</v>
       </c>
       <c r="L44" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>398.67566999999997</v>
+        <v>580.21711000000005</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="B45">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C45">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D45">
-        <v>29754</v>
+        <v>8080</v>
       </c>
       <c r="E45">
-        <v>29803</v>
+        <v>8112</v>
       </c>
       <c r="F45">
         <v>100</v>
@@ -3670,37 +3652,37 @@
         <v>12</v>
       </c>
       <c r="H45">
-        <v>5.45E-3</v>
+        <v>5.7499999999999999E-3</v>
       </c>
       <c r="I45">
-        <v>7.6740000000000003E-2</v>
+        <v>41.81</v>
       </c>
       <c r="J45">
-        <v>280.47131999999999</v>
+        <v>657.21583999999996</v>
       </c>
       <c r="K45">
-        <v>120.52744</v>
+        <v>1.58249</v>
       </c>
       <c r="L45" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>401.07549999999998</v>
+        <v>700.60833000000002</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="B46">
-        <v>64</v>
+        <v>1793</v>
       </c>
       <c r="C46">
-        <v>128</v>
+        <v>2305</v>
       </c>
       <c r="D46">
-        <v>29792</v>
+        <v>1330</v>
       </c>
       <c r="E46">
-        <v>29856</v>
+        <v>3123</v>
       </c>
       <c r="F46">
         <v>100</v>
@@ -3709,25 +3691,25 @@
         <v>12</v>
       </c>
       <c r="H46">
-        <v>6.1399999999999996E-3</v>
+        <v>1.8799999999999999E-3</v>
       </c>
       <c r="I46">
-        <v>30.743670000000002</v>
+        <v>41.837820000000001</v>
       </c>
       <c r="J46">
-        <v>385.53147000000001</v>
+        <v>9.6831999999999994</v>
       </c>
       <c r="K46">
-        <v>2.3719399999999999</v>
+        <v>9.0560000000000002E-2</v>
       </c>
       <c r="L46" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>418.64708000000002</v>
+        <v>51.611580000000004</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B47">
         <v>48</v>
@@ -3748,25 +3730,25 @@
         <v>12</v>
       </c>
       <c r="H47">
-        <v>4.9300000000000004E-3</v>
+        <v>5.8500000000000002E-3</v>
       </c>
       <c r="I47">
-        <v>16.841699999999999</v>
+        <v>47.65502</v>
       </c>
       <c r="J47">
-        <v>449.87601999999998</v>
+        <v>1005.47105</v>
       </c>
       <c r="K47">
-        <v>0.31336999999999998</v>
+        <v>3.5372499999999998</v>
       </c>
       <c r="L47" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>467.03109000000001</v>
+        <v>1056.6633200000001</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="B48">
         <v>48</v>
@@ -3787,25 +3769,25 @@
         <v>12</v>
       </c>
       <c r="H48">
-        <v>6.0600000000000003E-3</v>
+        <v>6.1799999999999997E-3</v>
       </c>
       <c r="I48">
-        <v>23.675170000000001</v>
+        <v>60.010210000000001</v>
       </c>
       <c r="J48">
-        <v>550.56377999999995</v>
+        <v>1371.74026</v>
       </c>
       <c r="K48">
-        <v>1.8194699999999999</v>
+        <v>2.3010000000000002</v>
       </c>
       <c r="L48" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>576.05841999999996</v>
+        <v>1434.0514699999999</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="B49">
         <v>32</v>
@@ -3826,37 +3808,37 @@
         <v>12</v>
       </c>
       <c r="H49">
-        <v>5.2199999999999998E-3</v>
+        <v>5.7499999999999999E-3</v>
       </c>
       <c r="I49">
-        <v>32.254190000000001</v>
+        <v>71.863299999999995</v>
       </c>
       <c r="J49">
-        <v>545.66493000000003</v>
+        <v>1075.28061</v>
       </c>
       <c r="K49">
-        <v>2.29799</v>
+        <v>3.0091600000000001</v>
       </c>
       <c r="L49" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>580.21711000000005</v>
+        <v>1150.1530700000001</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B50">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="C50">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="D50">
-        <v>8080</v>
+        <v>29792</v>
       </c>
       <c r="E50">
-        <v>8112</v>
+        <v>29856</v>
       </c>
       <c r="F50">
         <v>100</v>
@@ -3865,37 +3847,37 @@
         <v>12</v>
       </c>
       <c r="H50">
-        <v>5.7499999999999999E-3</v>
+        <v>6.5100000000000002E-3</v>
       </c>
       <c r="I50">
-        <v>41.81</v>
+        <v>76.74239</v>
       </c>
       <c r="J50">
-        <v>657.21583999999996</v>
+        <v>946.51715000000002</v>
       </c>
       <c r="K50">
-        <v>1.58249</v>
+        <v>2.99838</v>
       </c>
       <c r="L50" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>700.60833000000002</v>
+        <v>1026.25792</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="B51">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C51">
-        <v>97</v>
+        <v>128</v>
       </c>
       <c r="D51">
-        <v>54736</v>
+        <v>29792</v>
       </c>
       <c r="E51">
-        <v>54801</v>
+        <v>29856</v>
       </c>
       <c r="F51">
         <v>100</v>
@@ -3904,37 +3886,37 @@
         <v>12</v>
       </c>
       <c r="H51">
-        <v>6.0200000000000002E-3</v>
+        <v>5.7000000000000002E-3</v>
       </c>
       <c r="I51">
-        <v>8.1860000000000002E-2</v>
+        <v>104.81656</v>
       </c>
       <c r="J51">
-        <v>565.85675000000003</v>
+        <v>1204.7865400000001</v>
       </c>
       <c r="K51">
-        <v>210.28148999999999</v>
+        <v>5.3406099999999999</v>
       </c>
       <c r="L51" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>776.2201</v>
+        <v>1314.94371</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B52">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="C52">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="D52">
-        <v>29792</v>
+        <v>17064</v>
       </c>
       <c r="E52">
-        <v>29856</v>
+        <v>17112</v>
       </c>
       <c r="F52">
         <v>100</v>
@@ -3943,37 +3925,37 @@
         <v>12</v>
       </c>
       <c r="H52">
-        <v>6.5100000000000002E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="I52">
-        <v>76.74239</v>
+        <v>105.19821</v>
       </c>
       <c r="J52">
-        <v>946.51715000000002</v>
+        <v>2204.1916000000001</v>
       </c>
       <c r="K52">
-        <v>2.99838</v>
+        <v>4.3596899999999996</v>
       </c>
       <c r="L52" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>1026.25792</v>
+        <v>2313.7494999999999</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="B53">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C53">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="D53">
-        <v>17064</v>
+        <v>29792</v>
       </c>
       <c r="E53">
-        <v>17112</v>
+        <v>29856</v>
       </c>
       <c r="F53">
         <v>100</v>
@@ -3982,37 +3964,37 @@
         <v>12</v>
       </c>
       <c r="H53">
-        <v>5.8500000000000002E-3</v>
+        <v>6.4999999999999997E-3</v>
       </c>
       <c r="I53">
-        <v>47.65502</v>
+        <v>133.78276</v>
       </c>
       <c r="J53">
-        <v>1005.47105</v>
+        <v>1565.0881300000001</v>
       </c>
       <c r="K53">
-        <v>3.5372499999999998</v>
+        <v>5.6985099999999997</v>
       </c>
       <c r="L53" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>1056.6633200000001</v>
+        <v>1704.5694000000001</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="B54">
-        <v>32</v>
+        <v>148992</v>
       </c>
       <c r="C54">
+        <v>92960</v>
+      </c>
+      <c r="D54">
         <v>64</v>
       </c>
-      <c r="D54">
-        <v>8080</v>
-      </c>
       <c r="E54">
-        <v>8112</v>
+        <v>149056</v>
       </c>
       <c r="F54">
         <v>100</v>
@@ -4021,37 +4003,37 @@
         <v>12</v>
       </c>
       <c r="H54">
-        <v>5.7499999999999999E-3</v>
+        <v>1.3610000000000001E-2</v>
       </c>
       <c r="I54">
-        <v>71.863299999999995</v>
+        <v>168.57817</v>
       </c>
       <c r="J54">
-        <v>1075.28061</v>
+        <v>2.1260400000000002</v>
       </c>
       <c r="K54">
-        <v>3.0091600000000001</v>
+        <v>2.2493300000000001</v>
       </c>
       <c r="L54" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>1150.1530700000001</v>
+        <v>172.95353999999998</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="B55">
+        <v>58144</v>
+      </c>
+      <c r="C55">
         <v>64</v>
       </c>
-      <c r="C55">
-        <v>128</v>
-      </c>
       <c r="D55">
-        <v>29792</v>
+        <v>64</v>
       </c>
       <c r="E55">
-        <v>29856</v>
+        <v>58208</v>
       </c>
       <c r="F55">
         <v>100</v>
@@ -4060,37 +4042,37 @@
         <v>12</v>
       </c>
       <c r="H55">
-        <v>5.7000000000000002E-3</v>
+        <v>1.048E-2</v>
       </c>
       <c r="I55">
-        <v>104.81656</v>
+        <v>178.06133</v>
       </c>
       <c r="J55">
-        <v>1204.7865400000001</v>
+        <v>75.439949999999996</v>
       </c>
       <c r="K55">
-        <v>5.3406099999999999</v>
+        <v>2.6040700000000001</v>
       </c>
       <c r="L55" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>1314.94371</v>
+        <v>256.10534999999999</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="B56">
-        <v>48</v>
+        <v>58144</v>
       </c>
       <c r="C56">
-        <v>96</v>
+        <v>92960</v>
       </c>
       <c r="D56">
-        <v>17064</v>
+        <v>64</v>
       </c>
       <c r="E56">
-        <v>17112</v>
+        <v>58208</v>
       </c>
       <c r="F56">
         <v>100</v>
@@ -4099,20 +4081,20 @@
         <v>12</v>
       </c>
       <c r="H56">
-        <v>6.1799999999999997E-3</v>
+        <v>1.2460000000000001E-2</v>
       </c>
       <c r="I56">
-        <v>60.010210000000001</v>
+        <v>179.50781000000001</v>
       </c>
       <c r="J56">
-        <v>1371.74026</v>
+        <v>1.95381</v>
       </c>
       <c r="K56">
-        <v>2.3010000000000002</v>
+        <v>2.4868000000000001</v>
       </c>
       <c r="L56" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>1434.0514699999999</v>
+        <v>183.94842</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
@@ -4156,19 +4138,19 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="B58">
+        <v>206744</v>
+      </c>
+      <c r="C58">
         <v>64</v>
       </c>
-      <c r="C58">
-        <v>128</v>
-      </c>
       <c r="D58">
-        <v>29792</v>
+        <v>156</v>
       </c>
       <c r="E58">
-        <v>29856</v>
+        <v>206900</v>
       </c>
       <c r="F58">
         <v>100</v>
@@ -4177,20 +4159,20 @@
         <v>12</v>
       </c>
       <c r="H58">
-        <v>6.4999999999999997E-3</v>
+        <v>1.9230000000000001E-2</v>
       </c>
       <c r="I58">
-        <v>133.78276</v>
+        <v>1764.7177200000001</v>
       </c>
       <c r="J58">
-        <v>1565.0881300000001</v>
+        <v>845.51125000000002</v>
       </c>
       <c r="K58">
-        <v>5.6985099999999997</v>
+        <v>17.433520000000001</v>
       </c>
       <c r="L58" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>1704.5694000000001</v>
+        <v>2627.6624900000002</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
@@ -4234,19 +4216,19 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="B60">
-        <v>48</v>
+        <v>1705536</v>
       </c>
       <c r="C60">
-        <v>96</v>
+        <v>1227104</v>
       </c>
       <c r="D60">
-        <v>17064</v>
+        <v>204</v>
       </c>
       <c r="E60">
-        <v>17112</v>
+        <v>1705740</v>
       </c>
       <c r="F60">
         <v>100</v>
@@ -4255,37 +4237,37 @@
         <v>12</v>
       </c>
       <c r="H60">
-        <v>6.0000000000000001E-3</v>
+        <v>1.8579999999999999E-2</v>
       </c>
       <c r="I60">
-        <v>105.19821</v>
+        <v>4935.3847699999997</v>
       </c>
       <c r="J60">
-        <v>2204.1916000000001</v>
+        <v>32.048929999999999</v>
       </c>
       <c r="K60">
-        <v>4.3596899999999996</v>
+        <v>34.561639999999997</v>
       </c>
       <c r="L60" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>2313.7494999999999</v>
+        <v>5001.9953399999995</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B61">
-        <v>206744</v>
+        <v>491936</v>
       </c>
       <c r="C61">
-        <v>64</v>
+        <v>1227104</v>
       </c>
       <c r="D61">
-        <v>156</v>
+        <v>204</v>
       </c>
       <c r="E61">
-        <v>206900</v>
+        <v>492140</v>
       </c>
       <c r="F61">
         <v>100</v>
@@ -4294,37 +4276,37 @@
         <v>12</v>
       </c>
       <c r="H61">
-        <v>1.9230000000000001E-2</v>
+        <v>2.2239999999999999E-2</v>
       </c>
       <c r="I61">
-        <v>1764.7177200000001</v>
+        <v>5600.4545099999996</v>
       </c>
       <c r="J61">
-        <v>845.51125000000002</v>
+        <v>32.103090000000002</v>
       </c>
       <c r="K61">
-        <v>17.433520000000001</v>
+        <v>40.567410000000002</v>
       </c>
       <c r="L61" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>2627.6624900000002</v>
+        <v>5673.1250099999988</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B62">
-        <v>1705536</v>
+        <v>491936</v>
       </c>
       <c r="C62">
-        <v>1227104</v>
+        <v>64</v>
       </c>
       <c r="D62">
         <v>204</v>
       </c>
       <c r="E62">
-        <v>1705740</v>
+        <v>492140</v>
       </c>
       <c r="F62">
         <v>100</v>
@@ -4333,96 +4315,18 @@
         <v>12</v>
       </c>
       <c r="H62">
-        <v>1.8579999999999999E-2</v>
+        <v>2.0119999999999999E-2</v>
       </c>
       <c r="I62">
-        <v>4935.3847699999997</v>
+        <v>5610.2878499999997</v>
       </c>
       <c r="J62">
-        <v>32.048929999999999</v>
+        <v>2676.3595300000002</v>
       </c>
       <c r="K62">
-        <v>34.561639999999997</v>
+        <v>40.888159999999999</v>
       </c>
       <c r="L62" s="1">
-        <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>5001.9953399999995</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B63">
-        <v>491936</v>
-      </c>
-      <c r="C63">
-        <v>1227104</v>
-      </c>
-      <c r="D63">
-        <v>204</v>
-      </c>
-      <c r="E63">
-        <v>492140</v>
-      </c>
-      <c r="F63">
-        <v>100</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H63">
-        <v>2.2239999999999999E-2</v>
-      </c>
-      <c r="I63">
-        <v>5600.4545099999996</v>
-      </c>
-      <c r="J63">
-        <v>32.103090000000002</v>
-      </c>
-      <c r="K63">
-        <v>40.567410000000002</v>
-      </c>
-      <c r="L63" s="1">
-        <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
-        <v>5673.1250099999988</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B64">
-        <v>491936</v>
-      </c>
-      <c r="C64">
-        <v>64</v>
-      </c>
-      <c r="D64">
-        <v>204</v>
-      </c>
-      <c r="E64">
-        <v>492140</v>
-      </c>
-      <c r="F64">
-        <v>100</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H64">
-        <v>2.0119999999999999E-2</v>
-      </c>
-      <c r="I64">
-        <v>5610.2878499999997</v>
-      </c>
-      <c r="J64">
-        <v>2676.3595300000002</v>
-      </c>
-      <c r="K64">
-        <v>40.888159999999999</v>
-      </c>
-      <c r="L64" s="1">
         <f>Algorithm_benchmark_100[[#This Row],[Key generation milliseconds]]+Algorithm_benchmark_100[[#This Row],[Signing milliseconds]]+Algorithm_benchmark_100[[#This Row],[Verifying milliseconds]]</f>
         <v>8327.5355400000008</v>
       </c>

</xml_diff>